<commit_message>
Cambios generales, Actualizado, instalación de paquetes
</commit_message>
<xml_diff>
--- a/GEN_01_ConsultorIdealista/Data/Config.xlsx
+++ b/GEN_01_ConsultorIdealista/Data/Config.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocio\Documents\PDDIdealistaFinal\GEN_01_ConsultorIdealista\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F23EA9-659A-46DD-AFC0-57E23F27F71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="3330" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="3330" windowWidth="18000" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -166,12 +160,39 @@
   </si>
   <si>
     <t>El usuario de nuestra cuenta Outlook</t>
+  </si>
+  <si>
+    <t>Credenciales_ChatGPT</t>
+  </si>
+  <si>
+    <t>ProyectoRPA</t>
+  </si>
+  <si>
+    <t>Credenciales de Acceso para ChatGPT</t>
+  </si>
+  <si>
+    <t>DireccionURL</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/auth/login</t>
+  </si>
+  <si>
+    <t>Dirección de ChatGPT</t>
+  </si>
+  <si>
+    <t>DireccionURLIdealista</t>
+  </si>
+  <si>
+    <t>https://www.idealista.com/</t>
+  </si>
+  <si>
+    <t>Dirección de Idealista</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -296,7 +317,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -348,7 +369,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -542,18 +563,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -642,10 +663,42 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C10" s="4"/>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1637,15 +1690,17 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{3CE877BC-08D8-4A72-B23B-69D9E66A5B4E}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2808,7 +2863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Modificación Varia, tema de inicialización
</commit_message>
<xml_diff>
--- a/GEN_01_ConsultorIdealista/Data/Config.xlsx
+++ b/GEN_01_ConsultorIdealista/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Dirección de Idealista</t>
+  </si>
+  <si>
+    <t>Ruta_Prompt</t>
+  </si>
+  <si>
+    <t>"C:\Users\samue\Documents\PDDIdealistaFinal\GEN_01_ConsultorIdealista\Data\prompt_proyecto.txt"</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,7 +580,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -697,6 +703,12 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Integraciones en orden, del dispatcher, 1,2,3,4, algunas dudas en el ultimo.
</commit_message>
<xml_diff>
--- a/GEN_01_ConsultorIdealista/Data/Config.xlsx
+++ b/GEN_01_ConsultorIdealista/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -192,14 +192,38 @@
     <t>Ruta_Prompt</t>
   </si>
   <si>
-    <t>"C:\Users\samue\Documents\PDDIdealistaFinal\GEN_01_ConsultorIdealista\Data\prompt_proyecto.txt"</t>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>OrchestatorQueueFolder</t>
+  </si>
+  <si>
+    <t>ColaIdealista</t>
+  </si>
+  <si>
+    <t>ColaIdealista1</t>
+  </si>
+  <si>
+    <t>C:\Users\samue\Documents\PDDIdealistaFinal\GEN_01_ConsultorIdealista\Data\prompt_proyecto.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,6 +253,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +293,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -569,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,7 +612,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -707,32 +739,61 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Parte Dispatcher finalizada, empezando parte de Process
</commit_message>
<xml_diff>
--- a/GEN_01_ConsultorIdealista/Data/Config.xlsx
+++ b/GEN_01_ConsultorIdealista/Data/Config.xlsx
@@ -207,9 +207,6 @@
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>OrchestatorQueueFolder</t>
-  </si>
-  <si>
     <t>ColaIdealista</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>C:\Users\samue\Documents\PDDIdealistaFinal\GEN_01_ConsultorIdealista\Data\prompt_proyecto.txt</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,7 +612,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -739,7 +739,7 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -748,7 +748,7 @@
         <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>59</v>
@@ -768,10 +768,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
         <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>